<commit_message>
canalizador x localidad hecho
</commit_message>
<xml_diff>
--- a/BAJADA1 CRD 12-05.xlsx
+++ b/BAJADA1 CRD 12-05.xlsx
@@ -1,23 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rstaffolani\Desktop\unificar-archivos-ocasa\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\roman\OneDrive\Escritorio\unificar-archivos-ocasa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{661C247D-53EE-40BC-ABCC-396D4C5E249C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C381CAB-25D5-4EE7-9C03-C7E304541892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{55E180D5-7D6A-4F9D-BAAC-711259D56438}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{55E180D5-7D6A-4F9D-BAAC-711259D56438}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -1634,7 +1645,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="#,##0.000"/>
+    <numFmt numFmtId="164" formatCode="#,##0.000"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -2135,16 +2146,17 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2502,60 +2514,60 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB787ED4-792B-4945-ABCC-680025987E39}">
   <dimension ref="A1:AT73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="AG1" sqref="AG1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.08984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.90625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.81640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.6328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.26953125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.7265625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.90625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="38.6328125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="42.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="21" max="22" width="12" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="17.90625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="5.1796875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="30.90625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.81640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="8" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="6.90625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="18.90625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="7.26953125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="6.90625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="43.6328125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="5.08984375" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="12.54296875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="43.453125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="43.42578125" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="16" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="6.81640625" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="13.1796875" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="34.90625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="11.90625" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="34.85546875" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2574,7 +2586,7 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
@@ -2695,7 +2707,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>46</v>
       </c>
@@ -2805,7 +2817,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>74</v>
       </c>
@@ -2915,7 +2927,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="4" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>86</v>
       </c>
@@ -3025,7 +3037,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="5" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>90</v>
       </c>
@@ -3135,7 +3147,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>94</v>
       </c>
@@ -3245,7 +3257,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>98</v>
       </c>
@@ -3355,7 +3367,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>101</v>
       </c>
@@ -3465,7 +3477,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="9" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>104</v>
       </c>
@@ -3575,7 +3587,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>108</v>
       </c>
@@ -3685,7 +3697,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>111</v>
       </c>
@@ -3795,7 +3807,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="12" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>115</v>
       </c>
@@ -3905,7 +3917,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="13" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>118</v>
       </c>
@@ -4015,7 +4027,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>121</v>
       </c>
@@ -4125,7 +4137,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>124</v>
       </c>
@@ -4233,7 +4245,7 @@
       </c>
       <c r="AT15" s="1"/>
     </row>
-    <row r="16" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>139</v>
       </c>
@@ -4335,7 +4347,7 @@
       </c>
       <c r="AT16" s="1"/>
     </row>
-    <row r="17" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>146</v>
       </c>
@@ -4435,7 +4447,7 @@
       </c>
       <c r="AT17" s="1"/>
     </row>
-    <row r="18" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>154</v>
       </c>
@@ -4543,7 +4555,7 @@
       </c>
       <c r="AT18" s="1"/>
     </row>
-    <row r="19" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>165</v>
       </c>
@@ -4643,7 +4655,7 @@
       </c>
       <c r="AT19" s="1"/>
     </row>
-    <row r="20" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>173</v>
       </c>
@@ -4753,7 +4765,7 @@
       </c>
       <c r="AT20" s="1"/>
     </row>
-    <row r="21" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>183</v>
       </c>
@@ -4861,7 +4873,7 @@
       </c>
       <c r="AT21" s="1"/>
     </row>
-    <row r="22" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>190</v>
       </c>
@@ -4969,7 +4981,7 @@
       </c>
       <c r="AT22" s="1"/>
     </row>
-    <row r="23" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>198</v>
       </c>
@@ -5069,7 +5081,7 @@
       </c>
       <c r="AT23" s="1"/>
     </row>
-    <row r="24" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>202</v>
       </c>
@@ -5169,7 +5181,7 @@
       </c>
       <c r="AT24" s="1"/>
     </row>
-    <row r="25" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>207</v>
       </c>
@@ -5277,7 +5289,7 @@
       </c>
       <c r="AT25" s="1"/>
     </row>
-    <row r="26" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>214</v>
       </c>
@@ -5387,7 +5399,7 @@
       </c>
       <c r="AT26" s="1"/>
     </row>
-    <row r="27" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>223</v>
       </c>
@@ -5495,7 +5507,7 @@
       </c>
       <c r="AT27" s="1"/>
     </row>
-    <row r="28" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>230</v>
       </c>
@@ -5603,7 +5615,7 @@
       </c>
       <c r="AT28" s="1"/>
     </row>
-    <row r="29" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>237</v>
       </c>
@@ -5707,7 +5719,7 @@
       </c>
       <c r="AT29" s="1"/>
     </row>
-    <row r="30" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>242</v>
       </c>
@@ -5815,7 +5827,7 @@
       </c>
       <c r="AT30" s="1"/>
     </row>
-    <row r="31" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>251</v>
       </c>
@@ -5923,7 +5935,7 @@
       </c>
       <c r="AT31" s="1"/>
     </row>
-    <row r="32" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>258</v>
       </c>
@@ -6029,7 +6041,7 @@
       </c>
       <c r="AT32" s="1"/>
     </row>
-    <row r="33" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>268</v>
       </c>
@@ -6135,7 +6147,7 @@
       </c>
       <c r="AT33" s="1"/>
     </row>
-    <row r="34" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>277</v>
       </c>
@@ -6241,7 +6253,7 @@
       </c>
       <c r="AT34" s="1"/>
     </row>
-    <row r="35" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>285</v>
       </c>
@@ -6347,7 +6359,7 @@
       </c>
       <c r="AT35" s="1"/>
     </row>
-    <row r="36" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>288</v>
       </c>
@@ -6453,7 +6465,7 @@
       </c>
       <c r="AT36" s="1"/>
     </row>
-    <row r="37" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>291</v>
       </c>
@@ -6561,7 +6573,7 @@
       </c>
       <c r="AT37" s="1"/>
     </row>
-    <row r="38" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>300</v>
       </c>
@@ -6667,7 +6679,7 @@
       </c>
       <c r="AT38" s="1"/>
     </row>
-    <row r="39" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>308</v>
       </c>
@@ -6773,7 +6785,7 @@
       </c>
       <c r="AT39" s="1"/>
     </row>
-    <row r="40" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>316</v>
       </c>
@@ -6873,7 +6885,7 @@
       </c>
       <c r="AT40" s="1"/>
     </row>
-    <row r="41" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>325</v>
       </c>
@@ -6975,7 +6987,7 @@
       </c>
       <c r="AT41" s="1"/>
     </row>
-    <row r="42" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>335</v>
       </c>
@@ -7075,7 +7087,7 @@
       </c>
       <c r="AT42" s="1"/>
     </row>
-    <row r="43" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>343</v>
       </c>
@@ -7183,7 +7195,7 @@
       </c>
       <c r="AT43" s="1"/>
     </row>
-    <row r="44" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>353</v>
       </c>
@@ -7287,7 +7299,7 @@
       </c>
       <c r="AT44" s="1"/>
     </row>
-    <row r="45" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>358</v>
       </c>
@@ -7395,7 +7407,7 @@
       </c>
       <c r="AT45" s="1"/>
     </row>
-    <row r="46" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>363</v>
       </c>
@@ -7497,7 +7509,7 @@
       </c>
       <c r="AT46" s="1"/>
     </row>
-    <row r="47" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>369</v>
       </c>
@@ -7597,7 +7609,7 @@
       </c>
       <c r="AT47" s="1"/>
     </row>
-    <row r="48" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>372</v>
       </c>
@@ -7703,7 +7715,7 @@
       </c>
       <c r="AT48" s="1"/>
     </row>
-    <row r="49" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>384</v>
       </c>
@@ -7809,7 +7821,7 @@
       </c>
       <c r="AT49" s="1"/>
     </row>
-    <row r="50" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>393</v>
       </c>
@@ -7915,7 +7927,7 @@
       </c>
       <c r="AT50" s="1"/>
     </row>
-    <row r="51" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>397</v>
       </c>
@@ -8021,7 +8033,7 @@
       </c>
       <c r="AT51" s="1"/>
     </row>
-    <row r="52" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>407</v>
       </c>
@@ -8127,7 +8139,7 @@
       </c>
       <c r="AT52" s="1"/>
     </row>
-    <row r="53" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>413</v>
       </c>
@@ -8227,7 +8239,7 @@
       </c>
       <c r="AT53" s="1"/>
     </row>
-    <row r="54" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>418</v>
       </c>
@@ -8327,7 +8339,7 @@
       </c>
       <c r="AT54" s="1"/>
     </row>
-    <row r="55" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>420</v>
       </c>
@@ -8437,7 +8449,7 @@
       </c>
       <c r="AT55" s="1"/>
     </row>
-    <row r="56" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>433</v>
       </c>
@@ -8545,7 +8557,7 @@
       </c>
       <c r="AT56" s="1"/>
     </row>
-    <row r="57" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>443</v>
       </c>
@@ -8655,7 +8667,7 @@
       </c>
       <c r="AT57" s="1"/>
     </row>
-    <row r="58" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>450</v>
       </c>
@@ -8757,7 +8769,7 @@
       </c>
       <c r="AT58" s="1"/>
     </row>
-    <row r="59" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>454</v>
       </c>
@@ -8861,7 +8873,7 @@
       </c>
       <c r="AT59" s="1"/>
     </row>
-    <row r="60" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>462</v>
       </c>
@@ -8967,7 +8979,7 @@
       </c>
       <c r="AT60" s="1"/>
     </row>
-    <row r="61" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
         <v>470</v>
       </c>
@@ -9067,7 +9079,7 @@
       </c>
       <c r="AT61" s="1"/>
     </row>
-    <row r="62" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
         <v>475</v>
       </c>
@@ -9169,7 +9181,7 @@
       </c>
       <c r="AT62" s="1"/>
     </row>
-    <row r="63" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
         <v>481</v>
       </c>
@@ -9269,7 +9281,7 @@
       </c>
       <c r="AT63" s="1"/>
     </row>
-    <row r="64" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
         <v>485</v>
       </c>
@@ -9375,7 +9387,7 @@
       </c>
       <c r="AT64" s="1"/>
     </row>
-    <row r="65" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
         <v>495</v>
       </c>
@@ -9481,7 +9493,7 @@
       </c>
       <c r="AT65" s="1"/>
     </row>
-    <row r="66" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
         <v>503</v>
       </c>
@@ -9587,7 +9599,7 @@
       </c>
       <c r="AT66" s="1"/>
     </row>
-    <row r="67" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
         <v>506</v>
       </c>
@@ -9687,7 +9699,7 @@
       </c>
       <c r="AT67" s="1"/>
     </row>
-    <row r="68" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
         <v>511</v>
       </c>
@@ -9789,7 +9801,7 @@
       </c>
       <c r="AT68" s="1"/>
     </row>
-    <row r="69" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
         <v>514</v>
       </c>
@@ -9889,7 +9901,7 @@
       </c>
       <c r="AT69" s="1"/>
     </row>
-    <row r="70" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
         <v>521</v>
       </c>
@@ -9989,7 +10001,7 @@
       </c>
       <c r="AT70" s="1"/>
     </row>
-    <row r="71" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
         <v>525</v>
       </c>
@@ -10087,7 +10099,7 @@
       </c>
       <c r="AT71" s="1"/>
     </row>
-    <row r="72" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
         <v>529</v>
       </c>
@@ -10193,7 +10205,7 @@
       </c>
       <c r="AT72" s="1"/>
     </row>
-    <row r="73" spans="1:46" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
         <v>532</v>
       </c>
@@ -10311,7 +10323,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -10323,7 +10335,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>